<commit_message>
Date selector functioning correctly
</commit_message>
<xml_diff>
--- a/Year2_GERR_Timetable.xlsx
+++ b/Year2_GERR_Timetable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3057234\OneDrive - Queen's University Belfast\Documents\timetable-web-application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44381C42-D457-44A3-B2F8-536ACCA85370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15296B45-1D9B-4CBF-9860-4D36A68BA7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="24 Week Timetable" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6770" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6770" uniqueCount="496">
   <si>
     <t>Unit</t>
   </si>
@@ -1523,6 +1523,15 @@
   </si>
   <si>
     <t>Dural sinuses and ventricular system</t>
+  </si>
+  <si>
+    <t>A01</t>
+  </si>
+  <si>
+    <t>A02</t>
+  </si>
+  <si>
+    <t>A03</t>
   </si>
 </sst>
 </file>
@@ -2683,8 +2692,8 @@
   </sheetPr>
   <dimension ref="A1:AW802"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A795" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H796" sqref="H796"/>
+    <sheetView tabSelected="1" topLeftCell="A785" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H801" sqref="H801"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="50.15" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -36685,7 +36694,7 @@
         <v>127</v>
       </c>
       <c r="E793" s="15">
-        <v>45275</v>
+        <v>45410</v>
       </c>
       <c r="F793" s="16">
         <v>0.54166666666666663</v>
@@ -36727,7 +36736,7 @@
         <v>127</v>
       </c>
       <c r="E794" s="15">
-        <v>45040</v>
+        <v>45410</v>
       </c>
       <c r="F794" s="16">
         <v>0.54166666666666663</v>
@@ -36769,7 +36778,7 @@
         <v>127</v>
       </c>
       <c r="E795" s="15">
-        <v>45040</v>
+        <v>45410</v>
       </c>
       <c r="F795" s="16">
         <v>0.54166666666666663</v>
@@ -36811,7 +36820,7 @@
         <v>127</v>
       </c>
       <c r="E796" s="15">
-        <v>45040</v>
+        <v>45410</v>
       </c>
       <c r="F796" s="16">
         <v>0.58333333333333337</v>
@@ -36855,7 +36864,7 @@
         <v>127</v>
       </c>
       <c r="E797" s="15">
-        <v>45407</v>
+        <v>45410</v>
       </c>
       <c r="F797" s="16">
         <v>0.625</v>
@@ -36897,7 +36906,7 @@
         <v>127</v>
       </c>
       <c r="E798" s="15">
-        <v>45407</v>
+        <v>45411</v>
       </c>
       <c r="F798" s="16">
         <v>0.625</v>
@@ -36939,7 +36948,7 @@
         <v>127</v>
       </c>
       <c r="E799" s="15">
-        <v>45407</v>
+        <v>45411</v>
       </c>
       <c r="F799" s="16">
         <v>0.625</v>
@@ -36990,7 +36999,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="H800" s="6" t="s">
-        <v>16</v>
+        <v>495</v>
       </c>
       <c r="I800" s="14" t="s">
         <v>59</v>
@@ -37023,7 +37032,7 @@
         <v>127</v>
       </c>
       <c r="E801" s="15">
-        <v>45408</v>
+        <v>45411</v>
       </c>
       <c r="F801" s="16">
         <v>0.625</v>
@@ -37032,7 +37041,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="H801" s="6" t="s">
-        <v>16</v>
+        <v>494</v>
       </c>
       <c r="I801" s="14" t="s">
         <v>61</v>
@@ -37065,7 +37074,7 @@
         <v>127</v>
       </c>
       <c r="E802" s="15">
-        <v>45408</v>
+        <v>45411</v>
       </c>
       <c r="F802" s="16">
         <v>0.625</v>
@@ -37074,7 +37083,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="H802" s="6" t="s">
-        <v>16</v>
+        <v>493</v>
       </c>
       <c r="I802" s="14" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
Max/min dates; worked UI (WIP)
</commit_message>
<xml_diff>
--- a/Year2_GERR_Timetable.xlsx
+++ b/Year2_GERR_Timetable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3057234\OneDrive - Queen's University Belfast\Documents\timetable-web-application\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://qubstudentcloud-my.sharepoint.com/personal/3057234_ads_qub_ac_uk/Documents/Documents/timetable_web_application-master/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15296B45-1D9B-4CBF-9860-4D36A68BA7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{15296B45-1D9B-4CBF-9860-4D36A68BA7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90DACB44-8828-4218-AAC2-90FEA2A8CFD6}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="24 Week Timetable" sheetId="1" r:id="rId1"/>
@@ -2423,6 +2423,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2692,30 +2696,30 @@
   </sheetPr>
   <dimension ref="A1:AW802"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A785" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H801" sqref="H801"/>
+    <sheetView tabSelected="1" topLeftCell="A778" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G801" sqref="G801"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="50.15" customHeight="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.54296875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="9.26953125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="7.7265625" style="86" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="13.26953125" style="12" customWidth="1"/>
-    <col min="7" max="7" width="11.54296875" style="12" customWidth="1"/>
-    <col min="8" max="8" width="12.453125" style="9" customWidth="1"/>
-    <col min="9" max="9" width="17.7265625" style="79" customWidth="1"/>
-    <col min="10" max="10" width="16.54296875" style="7" customWidth="1"/>
-    <col min="11" max="11" width="20.453125" style="7" customWidth="1"/>
-    <col min="12" max="12" width="20.54296875" style="7" customWidth="1"/>
-    <col min="13" max="13" width="34.7265625" style="10" customWidth="1"/>
-    <col min="14" max="14" width="26.54296875" style="11" customWidth="1"/>
-    <col min="15" max="16384" width="8.54296875" style="7"/>
+    <col min="1" max="1" width="6.5703125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" style="86" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" style="79" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" style="7" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" style="7" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" style="7" customWidth="1"/>
+    <col min="13" max="13" width="34.7109375" style="10" customWidth="1"/>
+    <col min="14" max="14" width="26.5703125" style="11" customWidth="1"/>
+    <col min="15" max="16384" width="8.5703125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
@@ -2773,7 +2777,7 @@
         <v>15</v>
       </c>
       <c r="E2" s="46">
-        <v>45187</v>
+        <v>45413</v>
       </c>
       <c r="F2" s="16">
         <v>0.4375</v>
@@ -2815,7 +2819,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="46">
-        <v>45187</v>
+        <v>45413</v>
       </c>
       <c r="F3" s="16">
         <v>0.58333333333333337</v>
@@ -2859,7 +2863,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="46">
-        <v>45187</v>
+        <v>45413</v>
       </c>
       <c r="F4" s="16">
         <v>0.625</v>
@@ -2889,7 +2893,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A5" s="54" t="s">
         <v>14</v>
       </c>
@@ -2903,7 +2907,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="46">
-        <v>45187</v>
+        <v>45413</v>
       </c>
       <c r="F5" s="16">
         <v>0.66666666666666663</v>
@@ -2947,7 +2951,7 @@
         <v>36</v>
       </c>
       <c r="E6" s="46">
-        <v>45188</v>
+        <v>45413</v>
       </c>
       <c r="F6" s="16">
         <v>0.375</v>
@@ -2991,7 +2995,7 @@
         <v>36</v>
       </c>
       <c r="E7" s="46">
-        <v>45188</v>
+        <v>45413</v>
       </c>
       <c r="F7" s="16">
         <v>0.375</v>
@@ -3021,7 +3025,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A8" s="54" t="s">
         <v>14</v>
       </c>
@@ -3035,7 +3039,7 @@
         <v>36</v>
       </c>
       <c r="E8" s="46">
-        <v>45188</v>
+        <v>45413</v>
       </c>
       <c r="F8" s="16">
         <v>0.375</v>
@@ -3063,7 +3067,7 @@
       </c>
       <c r="N8" s="36"/>
     </row>
-    <row r="9" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A9" s="54" t="s">
         <v>14</v>
       </c>
@@ -3077,7 +3081,7 @@
         <v>36</v>
       </c>
       <c r="E9" s="46">
-        <v>45188</v>
+        <v>45413</v>
       </c>
       <c r="F9" s="16">
         <v>0.375</v>
@@ -3105,7 +3109,7 @@
       </c>
       <c r="N9" s="36"/>
     </row>
-    <row r="10" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A10" s="54" t="s">
         <v>14</v>
       </c>
@@ -3147,7 +3151,7 @@
       </c>
       <c r="N10" s="36"/>
     </row>
-    <row r="11" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A11" s="54" t="s">
         <v>14</v>
       </c>
@@ -3189,7 +3193,7 @@
       </c>
       <c r="N11" s="36"/>
     </row>
-    <row r="12" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A12" s="54" t="s">
         <v>14</v>
       </c>
@@ -3231,7 +3235,7 @@
       </c>
       <c r="N12" s="36"/>
     </row>
-    <row r="13" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A13" s="54" t="s">
         <v>14</v>
       </c>
@@ -3273,7 +3277,7 @@
       </c>
       <c r="N13" s="36"/>
     </row>
-    <row r="14" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A14" s="54" t="s">
         <v>14</v>
       </c>
@@ -3525,7 +3529,7 @@
       </c>
       <c r="N19" s="36"/>
     </row>
-    <row r="20" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A20" s="54" t="s">
         <v>14</v>
       </c>
@@ -3569,7 +3573,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A21" s="54" t="s">
         <v>14</v>
       </c>
@@ -3611,7 +3615,7 @@
       </c>
       <c r="N21" s="36"/>
     </row>
-    <row r="22" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A22" s="54" t="s">
         <v>14</v>
       </c>
@@ -3653,7 +3657,7 @@
       </c>
       <c r="N22" s="36"/>
     </row>
-    <row r="23" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A23" s="54" t="s">
         <v>14</v>
       </c>
@@ -3695,7 +3699,7 @@
       </c>
       <c r="N23" s="36"/>
     </row>
-    <row r="24" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A24" s="54" t="s">
         <v>14</v>
       </c>
@@ -3865,7 +3869,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A28" s="54" t="s">
         <v>14</v>
       </c>
@@ -3907,7 +3911,7 @@
       </c>
       <c r="N28" s="36"/>
     </row>
-    <row r="29" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A29" s="54" t="s">
         <v>14</v>
       </c>
@@ -3949,7 +3953,7 @@
       </c>
       <c r="N29" s="36"/>
     </row>
-    <row r="30" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A30" s="54" t="s">
         <v>14</v>
       </c>
@@ -3991,7 +3995,7 @@
       </c>
       <c r="N30" s="36"/>
     </row>
-    <row r="31" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A31" s="54" t="s">
         <v>14</v>
       </c>
@@ -4033,7 +4037,7 @@
       </c>
       <c r="N31" s="36"/>
     </row>
-    <row r="32" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A32" s="54" t="s">
         <v>14</v>
       </c>
@@ -4075,7 +4079,7 @@
       </c>
       <c r="N32" s="36"/>
     </row>
-    <row r="33" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A33" s="54" t="s">
         <v>14</v>
       </c>
@@ -4293,7 +4297,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A38" s="54" t="s">
         <v>14</v>
       </c>
@@ -4601,7 +4605,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A45" s="54" t="s">
         <v>14</v>
       </c>
@@ -4645,7 +4649,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A46" s="54" t="s">
         <v>14</v>
       </c>
@@ -4733,7 +4737,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A48" s="54" t="s">
         <v>14</v>
       </c>
@@ -4777,7 +4781,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A49" s="54" t="s">
         <v>14</v>
       </c>
@@ -4819,7 +4823,7 @@
       </c>
       <c r="N49" s="36"/>
     </row>
-    <row r="50" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A50" s="54" t="s">
         <v>14</v>
       </c>
@@ -4861,7 +4865,7 @@
       </c>
       <c r="N50" s="36"/>
     </row>
-    <row r="51" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A51" s="54" t="s">
         <v>14</v>
       </c>
@@ -4903,7 +4907,7 @@
       </c>
       <c r="N51" s="36"/>
     </row>
-    <row r="52" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A52" s="54" t="s">
         <v>14</v>
       </c>
@@ -4945,7 +4949,7 @@
       </c>
       <c r="N52" s="36"/>
     </row>
-    <row r="53" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A53" s="54" t="s">
         <v>14</v>
       </c>
@@ -4987,7 +4991,7 @@
       </c>
       <c r="N53" s="36"/>
     </row>
-    <row r="54" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A54" s="54" t="s">
         <v>14</v>
       </c>
@@ -5029,7 +5033,7 @@
       </c>
       <c r="N54" s="36"/>
     </row>
-    <row r="55" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A55" s="54" t="s">
         <v>14</v>
       </c>
@@ -5073,7 +5077,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A56" s="54" t="s">
         <v>14</v>
       </c>
@@ -5117,7 +5121,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A57" s="54" t="s">
         <v>14</v>
       </c>
@@ -5159,7 +5163,7 @@
       </c>
       <c r="N57" s="36"/>
     </row>
-    <row r="58" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A58" s="54" t="s">
         <v>14</v>
       </c>
@@ -5201,7 +5205,7 @@
       </c>
       <c r="N58" s="36"/>
     </row>
-    <row r="59" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A59" s="54" t="s">
         <v>14</v>
       </c>
@@ -5243,7 +5247,7 @@
       </c>
       <c r="N59" s="36"/>
     </row>
-    <row r="60" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A60" s="54" t="s">
         <v>14</v>
       </c>
@@ -5285,7 +5289,7 @@
       </c>
       <c r="N60" s="36"/>
     </row>
-    <row r="61" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A61" s="54" t="s">
         <v>14</v>
       </c>
@@ -5327,7 +5331,7 @@
       </c>
       <c r="N61" s="36"/>
     </row>
-    <row r="62" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A62" s="54" t="s">
         <v>14</v>
       </c>
@@ -5369,7 +5373,7 @@
       </c>
       <c r="N62" s="36"/>
     </row>
-    <row r="63" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A63" s="54" t="s">
         <v>14</v>
       </c>
@@ -5413,7 +5417,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A64" s="54" t="s">
         <v>14</v>
       </c>
@@ -5709,7 +5713,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A71" s="54" t="s">
         <v>14</v>
       </c>
@@ -5751,7 +5755,7 @@
       </c>
       <c r="N71" s="36"/>
     </row>
-    <row r="72" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A72" s="54" t="s">
         <v>14</v>
       </c>
@@ -5793,7 +5797,7 @@
       </c>
       <c r="N72" s="36"/>
     </row>
-    <row r="73" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A73" s="54" t="s">
         <v>14</v>
       </c>
@@ -5835,7 +5839,7 @@
       </c>
       <c r="N73" s="36"/>
     </row>
-    <row r="74" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A74" s="54" t="s">
         <v>14</v>
       </c>
@@ -6093,7 +6097,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="54" t="s">
         <v>14</v>
       </c>
@@ -6181,7 +6185,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A82" s="54" t="s">
         <v>14</v>
       </c>
@@ -6621,7 +6625,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="54" t="s">
         <v>14</v>
       </c>
@@ -6665,7 +6669,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A93" s="54" t="s">
         <v>14</v>
       </c>
@@ -6709,7 +6713,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="54" t="s">
         <v>14</v>
       </c>
@@ -6753,7 +6757,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="54" t="s">
         <v>14</v>
       </c>
@@ -6929,7 +6933,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A99" s="54" t="s">
         <v>14</v>
       </c>
@@ -6973,7 +6977,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A100" s="54" t="s">
         <v>14</v>
       </c>
@@ -7105,7 +7109,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A103" s="54" t="s">
         <v>14</v>
       </c>
@@ -7193,7 +7197,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A105" s="54" t="s">
         <v>14</v>
       </c>
@@ -7235,7 +7239,7 @@
       </c>
       <c r="N105" s="36"/>
     </row>
-    <row r="106" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A106" s="54" t="s">
         <v>14</v>
       </c>
@@ -7277,7 +7281,7 @@
       </c>
       <c r="N106" s="36"/>
     </row>
-    <row r="107" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A107" s="54" t="s">
         <v>14</v>
       </c>
@@ -7319,7 +7323,7 @@
       </c>
       <c r="N107" s="36"/>
     </row>
-    <row r="108" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A108" s="54" t="s">
         <v>14</v>
       </c>
@@ -7533,7 +7537,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A113" s="54" t="s">
         <v>14</v>
       </c>
@@ -7575,7 +7579,7 @@
       </c>
       <c r="N113" s="36"/>
     </row>
-    <row r="114" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A114" s="54" t="s">
         <v>14</v>
       </c>
@@ -7617,7 +7621,7 @@
       </c>
       <c r="N114" s="36"/>
     </row>
-    <row r="115" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A115" s="54" t="s">
         <v>14</v>
       </c>
@@ -7659,7 +7663,7 @@
       </c>
       <c r="N115" s="36"/>
     </row>
-    <row r="116" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A116" s="54" t="s">
         <v>14</v>
       </c>
@@ -7829,7 +7833,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A120" s="54" t="s">
         <v>14</v>
       </c>
@@ -7871,7 +7875,7 @@
       </c>
       <c r="N120" s="36"/>
     </row>
-    <row r="121" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A121" s="54" t="s">
         <v>14</v>
       </c>
@@ -7913,7 +7917,7 @@
       </c>
       <c r="N121" s="36"/>
     </row>
-    <row r="122" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A122" s="54" t="s">
         <v>14</v>
       </c>
@@ -7955,7 +7959,7 @@
       </c>
       <c r="N122" s="36"/>
     </row>
-    <row r="123" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A123" s="54" t="s">
         <v>14</v>
       </c>
@@ -7997,7 +8001,7 @@
       </c>
       <c r="N123" s="36"/>
     </row>
-    <row r="124" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A124" s="54" t="s">
         <v>14</v>
       </c>
@@ -8039,7 +8043,7 @@
       </c>
       <c r="N124" s="36"/>
     </row>
-    <row r="125" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A125" s="54" t="s">
         <v>14</v>
       </c>
@@ -8081,7 +8085,7 @@
       </c>
       <c r="N125" s="36"/>
     </row>
-    <row r="126" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A126" s="54" t="s">
         <v>14</v>
       </c>
@@ -8125,7 +8129,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A127" s="54" t="s">
         <v>14</v>
       </c>
@@ -8167,7 +8171,7 @@
       </c>
       <c r="N127" s="36"/>
     </row>
-    <row r="128" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A128" s="54" t="s">
         <v>14</v>
       </c>
@@ -8209,7 +8213,7 @@
       </c>
       <c r="N128" s="36"/>
     </row>
-    <row r="129" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A129" s="54" t="s">
         <v>14</v>
       </c>
@@ -8251,7 +8255,7 @@
       </c>
       <c r="N129" s="36"/>
     </row>
-    <row r="130" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A130" s="54" t="s">
         <v>14</v>
       </c>
@@ -8293,7 +8297,7 @@
       </c>
       <c r="N130" s="36"/>
     </row>
-    <row r="131" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A131" s="54" t="s">
         <v>14</v>
       </c>
@@ -8335,7 +8339,7 @@
       </c>
       <c r="N131" s="36"/>
     </row>
-    <row r="132" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A132" s="54" t="s">
         <v>14</v>
       </c>
@@ -8817,7 +8821,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="143" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A143" s="54" t="s">
         <v>14</v>
       </c>
@@ -8859,7 +8863,7 @@
       </c>
       <c r="N143" s="36"/>
     </row>
-    <row r="144" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A144" s="54" t="s">
         <v>14</v>
       </c>
@@ -8901,7 +8905,7 @@
       </c>
       <c r="N144" s="36"/>
     </row>
-    <row r="145" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A145" s="54" t="s">
         <v>14</v>
       </c>
@@ -8943,7 +8947,7 @@
       </c>
       <c r="N145" s="36"/>
     </row>
-    <row r="146" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A146" s="54" t="s">
         <v>14</v>
       </c>
@@ -8985,7 +8989,7 @@
       </c>
       <c r="N146" s="36"/>
     </row>
-    <row r="147" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A147" s="54" t="s">
         <v>14</v>
       </c>
@@ -9027,7 +9031,7 @@
       </c>
       <c r="N147" s="36"/>
     </row>
-    <row r="148" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A148" s="54" t="s">
         <v>14</v>
       </c>
@@ -9069,7 +9073,7 @@
       </c>
       <c r="N148" s="36"/>
     </row>
-    <row r="149" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A149" s="54" t="s">
         <v>14</v>
       </c>
@@ -9111,7 +9115,7 @@
       </c>
       <c r="N149" s="36"/>
     </row>
-    <row r="150" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A150" s="54" t="s">
         <v>14</v>
       </c>
@@ -9153,7 +9157,7 @@
       </c>
       <c r="N150" s="67"/>
     </row>
-    <row r="151" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A151" s="54" t="s">
         <v>14</v>
       </c>
@@ -9195,7 +9199,7 @@
       </c>
       <c r="N151" s="36"/>
     </row>
-    <row r="152" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A152" s="54" t="s">
         <v>14</v>
       </c>
@@ -9237,7 +9241,7 @@
       </c>
       <c r="N152" s="36"/>
     </row>
-    <row r="153" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A153" s="54" t="s">
         <v>14</v>
       </c>
@@ -9279,7 +9283,7 @@
       </c>
       <c r="N153" s="36"/>
     </row>
-    <row r="154" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A154" s="54" t="s">
         <v>14</v>
       </c>
@@ -9365,7 +9369,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="156" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A156" s="54" t="s">
         <v>14</v>
       </c>
@@ -9407,7 +9411,7 @@
       </c>
       <c r="N156" s="36"/>
     </row>
-    <row r="157" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A157" s="54" t="s">
         <v>14</v>
       </c>
@@ -9449,7 +9453,7 @@
       </c>
       <c r="N157" s="36"/>
     </row>
-    <row r="158" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A158" s="54" t="s">
         <v>14</v>
       </c>
@@ -9491,7 +9495,7 @@
       </c>
       <c r="N158" s="36"/>
     </row>
-    <row r="159" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A159" s="54" t="s">
         <v>14</v>
       </c>
@@ -9617,7 +9621,7 @@
       </c>
       <c r="N161" s="36"/>
     </row>
-    <row r="162" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A162" s="54" t="s">
         <v>14</v>
       </c>
@@ -9659,7 +9663,7 @@
       </c>
       <c r="N162" s="36"/>
     </row>
-    <row r="163" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A163" s="54" t="s">
         <v>14</v>
       </c>
@@ -9701,7 +9705,7 @@
       </c>
       <c r="N163" s="36"/>
     </row>
-    <row r="164" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A164" s="54" t="s">
         <v>14</v>
       </c>
@@ -9743,7 +9747,7 @@
       </c>
       <c r="N164" s="36"/>
     </row>
-    <row r="165" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A165" s="54" t="s">
         <v>14</v>
       </c>
@@ -10659,7 +10663,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="186" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A186" s="54" t="s">
         <v>14</v>
       </c>
@@ -10703,7 +10707,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="187" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A187" s="54" t="s">
         <v>14</v>
       </c>
@@ -10745,7 +10749,7 @@
       </c>
       <c r="N187" s="36"/>
     </row>
-    <row r="188" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A188" s="54" t="s">
         <v>14</v>
       </c>
@@ -10787,7 +10791,7 @@
       </c>
       <c r="N188" s="36"/>
     </row>
-    <row r="189" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A189" s="54" t="s">
         <v>14</v>
       </c>
@@ -10829,7 +10833,7 @@
       </c>
       <c r="N189" s="36"/>
     </row>
-    <row r="190" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A190" s="54" t="s">
         <v>14</v>
       </c>
@@ -10955,7 +10959,7 @@
       </c>
       <c r="N192" s="36"/>
     </row>
-    <row r="193" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A193" s="54" t="s">
         <v>14</v>
       </c>
@@ -11263,7 +11267,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="200" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A200" s="54" t="s">
         <v>14</v>
       </c>
@@ -11307,7 +11311,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="201" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A201" s="54" t="s">
         <v>14</v>
       </c>
@@ -11349,7 +11353,7 @@
       </c>
       <c r="N201" s="36"/>
     </row>
-    <row r="202" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A202" s="54" t="s">
         <v>14</v>
       </c>
@@ -11391,7 +11395,7 @@
       </c>
       <c r="N202" s="36"/>
     </row>
-    <row r="203" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A203" s="54" t="s">
         <v>14</v>
       </c>
@@ -11433,7 +11437,7 @@
       </c>
       <c r="N203" s="36"/>
     </row>
-    <row r="204" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A204" s="54" t="s">
         <v>14</v>
       </c>
@@ -11559,7 +11563,7 @@
       </c>
       <c r="N206" s="36"/>
     </row>
-    <row r="207" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A207" s="54" t="s">
         <v>14</v>
       </c>
@@ -11603,7 +11607,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="208" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A208" s="54" t="s">
         <v>14</v>
       </c>
@@ -11645,7 +11649,7 @@
       </c>
       <c r="N208" s="36"/>
     </row>
-    <row r="209" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A209" s="54" t="s">
         <v>14</v>
       </c>
@@ -11687,7 +11691,7 @@
       </c>
       <c r="N209" s="36"/>
     </row>
-    <row r="210" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A210" s="54" t="s">
         <v>14</v>
       </c>
@@ -11729,7 +11733,7 @@
       </c>
       <c r="N210" s="36"/>
     </row>
-    <row r="211" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A211" s="54" t="s">
         <v>14</v>
       </c>
@@ -11771,7 +11775,7 @@
       </c>
       <c r="N211" s="36"/>
     </row>
-    <row r="212" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A212" s="54" t="s">
         <v>14</v>
       </c>
@@ -11813,7 +11817,7 @@
       </c>
       <c r="N212" s="36"/>
     </row>
-    <row r="213" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A213" s="54" t="s">
         <v>14</v>
       </c>
@@ -11899,7 +11903,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="215" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A215" s="54" t="s">
         <v>14</v>
       </c>
@@ -11941,7 +11945,7 @@
       </c>
       <c r="N215" s="36"/>
     </row>
-    <row r="216" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A216" s="54" t="s">
         <v>14</v>
       </c>
@@ -11983,7 +11987,7 @@
       </c>
       <c r="N216" s="67"/>
     </row>
-    <row r="217" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A217" s="54" t="s">
         <v>14</v>
       </c>
@@ -12025,7 +12029,7 @@
       </c>
       <c r="N217" s="36"/>
     </row>
-    <row r="218" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A218" s="54" t="s">
         <v>14</v>
       </c>
@@ -12067,7 +12071,7 @@
       </c>
       <c r="N218" s="36"/>
     </row>
-    <row r="219" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A219" s="54" t="s">
         <v>14</v>
       </c>
@@ -12109,7 +12113,7 @@
       </c>
       <c r="N219" s="36"/>
     </row>
-    <row r="220" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A220" s="54" t="s">
         <v>14</v>
       </c>
@@ -13383,7 +13387,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="249" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A249" s="54" t="s">
         <v>14</v>
       </c>
@@ -13427,7 +13431,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="250" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A250" s="54" t="s">
         <v>14</v>
       </c>
@@ -13469,7 +13473,7 @@
       </c>
       <c r="N250" s="36"/>
     </row>
-    <row r="251" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A251" s="54" t="s">
         <v>14</v>
       </c>
@@ -13511,7 +13515,7 @@
       </c>
       <c r="N251" s="67"/>
     </row>
-    <row r="252" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A252" s="54" t="s">
         <v>14</v>
       </c>
@@ -13553,7 +13557,7 @@
       </c>
       <c r="N252" s="36"/>
     </row>
-    <row r="253" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A253" s="54" t="s">
         <v>14</v>
       </c>
@@ -13595,7 +13599,7 @@
       </c>
       <c r="N253" s="36"/>
     </row>
-    <row r="254" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A254" s="54" t="s">
         <v>14</v>
       </c>
@@ -13637,7 +13641,7 @@
       </c>
       <c r="N254" s="36"/>
     </row>
-    <row r="255" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A255" s="54" t="s">
         <v>14</v>
       </c>
@@ -13679,7 +13683,7 @@
       </c>
       <c r="N255" s="67"/>
     </row>
-    <row r="256" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A256" s="54" t="s">
         <v>14</v>
       </c>
@@ -13855,7 +13859,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="260" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A260" s="54" t="s">
         <v>14</v>
       </c>
@@ -14031,7 +14035,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="264" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A264" s="54" t="s">
         <v>14</v>
       </c>
@@ -14073,7 +14077,7 @@
       </c>
       <c r="N264" s="36"/>
     </row>
-    <row r="265" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A265" s="54" t="s">
         <v>14</v>
       </c>
@@ -14115,7 +14119,7 @@
       </c>
       <c r="N265" s="36"/>
     </row>
-    <row r="266" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A266" s="54" t="s">
         <v>14</v>
       </c>
@@ -14157,7 +14161,7 @@
       </c>
       <c r="N266" s="36"/>
     </row>
-    <row r="267" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A267" s="54" t="s">
         <v>14</v>
       </c>
@@ -14199,7 +14203,7 @@
       </c>
       <c r="N267" s="36"/>
     </row>
-    <row r="268" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A268" s="54" t="s">
         <v>14</v>
       </c>
@@ -14241,7 +14245,7 @@
       </c>
       <c r="N268" s="36"/>
     </row>
-    <row r="269" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A269" s="54" t="s">
         <v>14</v>
       </c>
@@ -14283,7 +14287,7 @@
       </c>
       <c r="N269" s="36"/>
     </row>
-    <row r="270" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A270" s="54" t="s">
         <v>14</v>
       </c>
@@ -14963,7 +14967,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="286" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A286" s="54" t="s">
         <v>14</v>
       </c>
@@ -15305,7 +15309,7 @@
       </c>
       <c r="N293" s="36"/>
     </row>
-    <row r="294" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A294" s="54" t="s">
         <v>14</v>
       </c>
@@ -15347,7 +15351,7 @@
       </c>
       <c r="N294" s="36"/>
     </row>
-    <row r="295" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A295" s="54" t="s">
         <v>14</v>
       </c>
@@ -16713,7 +16717,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="327" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A327" s="54" t="s">
         <v>14</v>
       </c>
@@ -17097,7 +17101,7 @@
       </c>
       <c r="N335" s="36"/>
     </row>
-    <row r="336" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A336" s="54" t="s">
         <v>14</v>
       </c>
@@ -19683,7 +19687,7 @@
       </c>
       <c r="N395" s="36"/>
     </row>
-    <row r="396" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A396" s="54" t="s">
         <v>14</v>
       </c>
@@ -19727,7 +19731,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="397" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A397" s="54" t="s">
         <v>14</v>
       </c>
@@ -20035,7 +20039,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="404" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A404" s="54" t="s">
         <v>14</v>
       </c>
@@ -20331,7 +20335,7 @@
       </c>
       <c r="N410" s="36"/>
     </row>
-    <row r="411" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A411" s="54" t="s">
         <v>14</v>
       </c>
@@ -21525,7 +21529,7 @@
       </c>
       <c r="N438" s="36"/>
     </row>
-    <row r="439" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A439" s="54" t="s">
         <v>14</v>
       </c>
@@ -22115,7 +22119,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="453" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A453" s="54" t="s">
         <v>14</v>
       </c>
@@ -22157,7 +22161,7 @@
       </c>
       <c r="N453" s="36"/>
     </row>
-    <row r="454" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A454" s="54" t="s">
         <v>14</v>
       </c>
@@ -22199,7 +22203,7 @@
       </c>
       <c r="N454" s="36"/>
     </row>
-    <row r="455" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A455" s="54" t="s">
         <v>14</v>
       </c>
@@ -22241,7 +22245,7 @@
       </c>
       <c r="N455" s="36"/>
     </row>
-    <row r="456" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A456" s="54" t="s">
         <v>14</v>
       </c>
@@ -22283,7 +22287,7 @@
       </c>
       <c r="N456" s="36"/>
     </row>
-    <row r="457" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A457" s="54" t="s">
         <v>14</v>
       </c>
@@ -22325,7 +22329,7 @@
       </c>
       <c r="N457" s="36"/>
     </row>
-    <row r="458" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A458" s="54" t="s">
         <v>14</v>
       </c>
@@ -22761,7 +22765,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="468" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A468" s="54" t="s">
         <v>14</v>
       </c>
@@ -23409,7 +23413,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="483" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A483" s="54" t="s">
         <v>14</v>
       </c>
@@ -23451,7 +23455,7 @@
       </c>
       <c r="N483" s="36"/>
     </row>
-    <row r="484" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A484" s="54" t="s">
         <v>14</v>
       </c>
@@ -23493,7 +23497,7 @@
       </c>
       <c r="N484" s="36"/>
     </row>
-    <row r="485" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A485" s="54" t="s">
         <v>14</v>
       </c>
@@ -23535,7 +23539,7 @@
       </c>
       <c r="N485" s="36"/>
     </row>
-    <row r="486" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A486" s="54" t="s">
         <v>14</v>
       </c>
@@ -23577,7 +23581,7 @@
       </c>
       <c r="N486" s="36"/>
     </row>
-    <row r="487" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A487" s="54" t="s">
         <v>14</v>
       </c>
@@ -23619,7 +23623,7 @@
       </c>
       <c r="N487" s="36"/>
     </row>
-    <row r="488" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A488" s="54" t="s">
         <v>14</v>
       </c>
@@ -23957,7 +23961,7 @@
       </c>
       <c r="N495" s="36"/>
     </row>
-    <row r="496" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A496" s="54" t="s">
         <v>14</v>
       </c>
@@ -24515,7 +24519,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="509" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="509" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A509" s="54" t="s">
         <v>14</v>
       </c>
@@ -24821,7 +24825,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="516" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="516" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A516" s="54" t="s">
         <v>14</v>
       </c>
@@ -24995,7 +24999,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="520" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="520" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A520" s="54" t="s">
         <v>14</v>
       </c>
@@ -25974,7 +25978,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="542" spans="1:49" ht="21" x14ac:dyDescent="0.25">
+    <row r="542" spans="1:49" ht="21" x14ac:dyDescent="0.2">
       <c r="A542" s="109" t="s">
         <v>14</v>
       </c>
@@ -26016,7 +26020,7 @@
       </c>
       <c r="N542" s="36"/>
     </row>
-    <row r="543" spans="1:49" ht="21" x14ac:dyDescent="0.25">
+    <row r="543" spans="1:49" ht="21" x14ac:dyDescent="0.2">
       <c r="A543" s="54" t="s">
         <v>14</v>
       </c>
@@ -26058,7 +26062,7 @@
       </c>
       <c r="N543" s="36"/>
     </row>
-    <row r="544" spans="1:49" ht="21" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:49" ht="21" x14ac:dyDescent="0.2">
       <c r="A544" s="54" t="s">
         <v>14</v>
       </c>
@@ -26100,7 +26104,7 @@
       </c>
       <c r="N544" s="36"/>
     </row>
-    <row r="545" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="545" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A545" s="54" t="s">
         <v>14</v>
       </c>
@@ -26142,7 +26146,7 @@
       </c>
       <c r="N545" s="36"/>
     </row>
-    <row r="546" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="546" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A546" s="54" t="s">
         <v>14</v>
       </c>
@@ -26184,7 +26188,7 @@
       </c>
       <c r="N546" s="36"/>
     </row>
-    <row r="547" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="547" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A547" s="54" t="s">
         <v>14</v>
       </c>
@@ -26270,7 +26274,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="549" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="549" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A549" s="54" t="s">
         <v>14</v>
       </c>
@@ -26312,7 +26316,7 @@
       </c>
       <c r="N549" s="36"/>
     </row>
-    <row r="550" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="550" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A550" s="54" t="s">
         <v>14</v>
       </c>
@@ -26354,7 +26358,7 @@
       </c>
       <c r="N550" s="36"/>
     </row>
-    <row r="551" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="551" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A551" s="54" t="s">
         <v>14</v>
       </c>
@@ -26396,7 +26400,7 @@
       </c>
       <c r="N551" s="36"/>
     </row>
-    <row r="552" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="552" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A552" s="54" t="s">
         <v>14</v>
       </c>
@@ -26438,7 +26442,7 @@
       </c>
       <c r="N552" s="36"/>
     </row>
-    <row r="553" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="553" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A553" s="54" t="s">
         <v>14</v>
       </c>
@@ -26480,7 +26484,7 @@
       </c>
       <c r="N553" s="36"/>
     </row>
-    <row r="554" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="554" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A554" s="54" t="s">
         <v>14</v>
       </c>
@@ -26642,7 +26646,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="558" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="558" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A558" s="54" t="s">
         <v>14</v>
       </c>
@@ -26682,7 +26686,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="559" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="559" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A559" s="54" t="s">
         <v>14</v>
       </c>
@@ -26722,7 +26726,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="560" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="560" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A560" s="138" t="s">
         <v>412</v>
       </c>
@@ -26810,7 +26814,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="562" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="562" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A562" s="138" t="s">
         <v>412</v>
       </c>
@@ -26854,7 +26858,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="563" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="563" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A563" s="138" t="s">
         <v>412</v>
       </c>
@@ -26898,7 +26902,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="564" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="564" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A564" s="138" t="s">
         <v>412</v>
       </c>
@@ -26940,7 +26944,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="565" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="565" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A565" s="138" t="s">
         <v>412</v>
       </c>
@@ -26982,7 +26986,7 @@
       </c>
       <c r="N565" s="36"/>
     </row>
-    <row r="566" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="566" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A566" s="138" t="s">
         <v>412</v>
       </c>
@@ -27024,7 +27028,7 @@
       </c>
       <c r="N566" s="36"/>
     </row>
-    <row r="567" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="567" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A567" s="138" t="s">
         <v>412</v>
       </c>
@@ -27066,7 +27070,7 @@
       </c>
       <c r="N567" s="36"/>
     </row>
-    <row r="568" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="568" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A568" s="138" t="s">
         <v>412</v>
       </c>
@@ -27108,7 +27112,7 @@
       </c>
       <c r="N568" s="36"/>
     </row>
-    <row r="569" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="569" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A569" s="138" t="s">
         <v>412</v>
       </c>
@@ -27150,7 +27154,7 @@
       </c>
       <c r="N569" s="36"/>
     </row>
-    <row r="570" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="570" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A570" s="138" t="s">
         <v>412</v>
       </c>
@@ -27192,7 +27196,7 @@
       </c>
       <c r="N570" s="36"/>
     </row>
-    <row r="571" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="571" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A571" s="138" t="s">
         <v>412</v>
       </c>
@@ -27234,7 +27238,7 @@
       </c>
       <c r="N571" s="36"/>
     </row>
-    <row r="572" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="572" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A572" s="138" t="s">
         <v>412</v>
       </c>
@@ -27276,7 +27280,7 @@
       </c>
       <c r="N572" s="36"/>
     </row>
-    <row r="573" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="573" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A573" s="138" t="s">
         <v>412</v>
       </c>
@@ -27318,7 +27322,7 @@
       </c>
       <c r="N573" s="36"/>
     </row>
-    <row r="574" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="574" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A574" s="138" t="s">
         <v>412</v>
       </c>
@@ -27360,7 +27364,7 @@
       </c>
       <c r="N574" s="36"/>
     </row>
-    <row r="575" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="575" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A575" s="138" t="s">
         <v>412</v>
       </c>
@@ -27402,7 +27406,7 @@
       </c>
       <c r="N575" s="36"/>
     </row>
-    <row r="576" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="576" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A576" s="138" t="s">
         <v>412</v>
       </c>
@@ -27444,7 +27448,7 @@
       </c>
       <c r="N576" s="36"/>
     </row>
-    <row r="577" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="577" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A577" s="138" t="s">
         <v>412</v>
       </c>
@@ -27486,7 +27490,7 @@
       </c>
       <c r="N577" s="36"/>
     </row>
-    <row r="578" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="578" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A578" s="138" t="s">
         <v>412</v>
       </c>
@@ -27528,7 +27532,7 @@
       </c>
       <c r="N578" s="36"/>
     </row>
-    <row r="579" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="579" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A579" s="138" t="s">
         <v>412</v>
       </c>
@@ -27570,7 +27574,7 @@
       </c>
       <c r="N579" s="36"/>
     </row>
-    <row r="580" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="580" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A580" s="138" t="s">
         <v>412</v>
       </c>
@@ -27612,7 +27616,7 @@
       </c>
       <c r="N580" s="36"/>
     </row>
-    <row r="581" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="581" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A581" s="138" t="s">
         <v>412</v>
       </c>
@@ -27654,7 +27658,7 @@
       </c>
       <c r="N581" s="36"/>
     </row>
-    <row r="582" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="582" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A582" s="138" t="s">
         <v>412</v>
       </c>
@@ -27696,7 +27700,7 @@
       </c>
       <c r="N582" s="36"/>
     </row>
-    <row r="583" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="583" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A583" s="138" t="s">
         <v>412</v>
       </c>
@@ -27738,7 +27742,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="584" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="584" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A584" s="138" t="s">
         <v>412</v>
       </c>
@@ -27780,7 +27784,7 @@
       </c>
       <c r="N584" s="36"/>
     </row>
-    <row r="585" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="585" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A585" s="138" t="s">
         <v>412</v>
       </c>
@@ -27822,7 +27826,7 @@
       </c>
       <c r="N585" s="36"/>
     </row>
-    <row r="586" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="586" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A586" s="138" t="s">
         <v>412</v>
       </c>
@@ -27864,7 +27868,7 @@
       </c>
       <c r="N586" s="36"/>
     </row>
-    <row r="587" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="587" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A587" s="138" t="s">
         <v>412</v>
       </c>
@@ -27906,7 +27910,7 @@
       </c>
       <c r="N587" s="36"/>
     </row>
-    <row r="588" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="588" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A588" s="138" t="s">
         <v>412</v>
       </c>
@@ -27948,7 +27952,7 @@
       </c>
       <c r="N588" s="36"/>
     </row>
-    <row r="589" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="589" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A589" s="138" t="s">
         <v>412</v>
       </c>
@@ -27990,7 +27994,7 @@
       </c>
       <c r="N589" s="36"/>
     </row>
-    <row r="590" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="590" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A590" s="138" t="s">
         <v>412</v>
       </c>
@@ -28034,7 +28038,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="591" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="591" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A591" s="138" t="s">
         <v>412</v>
       </c>
@@ -28078,7 +28082,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="592" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="592" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A592" s="138" t="s">
         <v>412</v>
       </c>
@@ -28122,7 +28126,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="593" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="593" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A593" s="138" t="s">
         <v>412</v>
       </c>
@@ -28166,7 +28170,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="594" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="594" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A594" s="138" t="s">
         <v>412</v>
       </c>
@@ -28208,7 +28212,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="595" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="595" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A595" s="138" t="s">
         <v>412</v>
       </c>
@@ -28252,7 +28256,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="596" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="596" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A596" s="138" t="s">
         <v>412</v>
       </c>
@@ -28296,7 +28300,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="597" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="597" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A597" s="138" t="s">
         <v>412</v>
       </c>
@@ -28340,7 +28344,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="598" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="598" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A598" s="138" t="s">
         <v>412</v>
       </c>
@@ -28384,7 +28388,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="599" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="599" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A599" s="138" t="s">
         <v>412</v>
       </c>
@@ -28428,7 +28432,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="600" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="600" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A600" s="138" t="s">
         <v>412</v>
       </c>
@@ -28516,7 +28520,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="602" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="602" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A602" s="138" t="s">
         <v>412</v>
       </c>
@@ -28558,7 +28562,7 @@
       </c>
       <c r="N602" s="36"/>
     </row>
-    <row r="603" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="603" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A603" s="138" t="s">
         <v>412</v>
       </c>
@@ -28600,7 +28604,7 @@
       </c>
       <c r="N603" s="36"/>
     </row>
-    <row r="604" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="604" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A604" s="138" t="s">
         <v>412</v>
       </c>
@@ -28642,7 +28646,7 @@
       </c>
       <c r="N604" s="36"/>
     </row>
-    <row r="605" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="605" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A605" s="138" t="s">
         <v>412</v>
       </c>
@@ -28684,7 +28688,7 @@
       </c>
       <c r="N605" s="36"/>
     </row>
-    <row r="606" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="606" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A606" s="138" t="s">
         <v>412</v>
       </c>
@@ -28726,7 +28730,7 @@
       </c>
       <c r="N606" s="36"/>
     </row>
-    <row r="607" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="607" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A607" s="138" t="s">
         <v>412</v>
       </c>
@@ -28856,7 +28860,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="610" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="610" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A610" s="138" t="s">
         <v>412</v>
       </c>
@@ -28898,7 +28902,7 @@
       </c>
       <c r="N610" s="39"/>
     </row>
-    <row r="611" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="611" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A611" s="138" t="s">
         <v>412</v>
       </c>
@@ -28940,7 +28944,7 @@
       </c>
       <c r="N611" s="36"/>
     </row>
-    <row r="612" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="612" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A612" s="138" t="s">
         <v>412</v>
       </c>
@@ -28982,7 +28986,7 @@
       </c>
       <c r="N612" s="39"/>
     </row>
-    <row r="613" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="613" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A613" s="138" t="s">
         <v>412</v>
       </c>
@@ -29024,7 +29028,7 @@
       </c>
       <c r="N613" s="39"/>
     </row>
-    <row r="614" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="614" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A614" s="138" t="s">
         <v>412</v>
       </c>
@@ -29066,7 +29070,7 @@
       </c>
       <c r="N614" s="39"/>
     </row>
-    <row r="615" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="615" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A615" s="138" t="s">
         <v>412</v>
       </c>
@@ -29152,7 +29156,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="617" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="617" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A617" s="138" t="s">
         <v>412</v>
       </c>
@@ -29194,7 +29198,7 @@
       </c>
       <c r="N617" s="36"/>
     </row>
-    <row r="618" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="618" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A618" s="138" t="s">
         <v>412</v>
       </c>
@@ -29236,7 +29240,7 @@
       </c>
       <c r="N618" s="36"/>
     </row>
-    <row r="619" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="619" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A619" s="138" t="s">
         <v>412</v>
       </c>
@@ -29278,7 +29282,7 @@
       </c>
       <c r="N619" s="39"/>
     </row>
-    <row r="620" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="620" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A620" s="138" t="s">
         <v>412</v>
       </c>
@@ -29320,7 +29324,7 @@
       </c>
       <c r="N620" s="39"/>
     </row>
-    <row r="621" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="621" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A621" s="138" t="s">
         <v>412</v>
       </c>
@@ -29362,7 +29366,7 @@
       </c>
       <c r="N621" s="36"/>
     </row>
-    <row r="622" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="622" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A622" s="138" t="s">
         <v>412</v>
       </c>
@@ -29404,7 +29408,7 @@
       </c>
       <c r="N622" s="36"/>
     </row>
-    <row r="623" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="623" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A623" s="138" t="s">
         <v>412</v>
       </c>
@@ -29448,7 +29452,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="624" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="624" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A624" s="138" t="s">
         <v>412</v>
       </c>
@@ -29490,7 +29494,7 @@
       </c>
       <c r="N624" s="36"/>
     </row>
-    <row r="625" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="625" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A625" s="138" t="s">
         <v>412</v>
       </c>
@@ -29532,7 +29536,7 @@
       </c>
       <c r="N625" s="36"/>
     </row>
-    <row r="626" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="626" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A626" s="138" t="s">
         <v>412</v>
       </c>
@@ -29574,7 +29578,7 @@
       </c>
       <c r="N626" s="36"/>
     </row>
-    <row r="627" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="627" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A627" s="138" t="s">
         <v>412</v>
       </c>
@@ -29616,7 +29620,7 @@
       </c>
       <c r="N627" s="36"/>
     </row>
-    <row r="628" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="628" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A628" s="138" t="s">
         <v>412</v>
       </c>
@@ -29658,7 +29662,7 @@
       </c>
       <c r="N628" s="36"/>
     </row>
-    <row r="629" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="629" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A629" s="138" t="s">
         <v>412</v>
       </c>
@@ -29744,7 +29748,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="631" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="631" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A631" s="138" t="s">
         <v>412</v>
       </c>
@@ -29788,7 +29792,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="632" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="632" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A632" s="138" t="s">
         <v>412</v>
       </c>
@@ -29832,7 +29836,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="633" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="633" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A633" s="138" t="s">
         <v>412</v>
       </c>
@@ -29876,7 +29880,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="634" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="634" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A634" s="138" t="s">
         <v>412</v>
       </c>
@@ -29920,7 +29924,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="635" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="635" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A635" s="138" t="s">
         <v>412</v>
       </c>
@@ -29964,7 +29968,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="636" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="636" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A636" s="138" t="s">
         <v>412</v>
       </c>
@@ -30050,7 +30054,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="638" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="638" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A638" s="138" t="s">
         <v>412</v>
       </c>
@@ -30094,7 +30098,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="639" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="639" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A639" s="138" t="s">
         <v>412</v>
       </c>
@@ -30136,7 +30140,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="640" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="640" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A640" s="138" t="s">
         <v>412</v>
       </c>
@@ -30180,7 +30184,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="641" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="641" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A641" s="138" t="s">
         <v>412</v>
       </c>
@@ -30224,7 +30228,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="642" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="642" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A642" s="138" t="s">
         <v>412</v>
       </c>
@@ -30268,7 +30272,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="643" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="643" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A643" s="138" t="s">
         <v>412</v>
       </c>
@@ -30312,7 +30316,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="644" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="644" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A644" s="138" t="s">
         <v>412</v>
       </c>
@@ -30356,7 +30360,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="645" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="645" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A645" s="138" t="s">
         <v>412</v>
       </c>
@@ -30400,7 +30404,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="646" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="646" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A646" s="138" t="s">
         <v>412</v>
       </c>
@@ -30442,7 +30446,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="647" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="647" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A647" s="138" t="s">
         <v>412</v>
       </c>
@@ -30486,7 +30490,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="648" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="648" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A648" s="138" t="s">
         <v>412</v>
       </c>
@@ -30530,7 +30534,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="649" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="649" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A649" s="138" t="s">
         <v>412</v>
       </c>
@@ -30618,7 +30622,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="651" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="651" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A651" s="138" t="s">
         <v>412</v>
       </c>
@@ -30706,7 +30710,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="653" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="653" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A653" s="138" t="s">
         <v>412</v>
       </c>
@@ -30748,7 +30752,7 @@
       </c>
       <c r="N653" s="36"/>
     </row>
-    <row r="654" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="654" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A654" s="138" t="s">
         <v>412</v>
       </c>
@@ -30790,7 +30794,7 @@
       </c>
       <c r="N654" s="36"/>
     </row>
-    <row r="655" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="655" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A655" s="138" t="s">
         <v>412</v>
       </c>
@@ -30832,7 +30836,7 @@
       </c>
       <c r="N655" s="36"/>
     </row>
-    <row r="656" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="656" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A656" s="138" t="s">
         <v>412</v>
       </c>
@@ -30874,7 +30878,7 @@
       </c>
       <c r="N656" s="36"/>
     </row>
-    <row r="657" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="657" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A657" s="138" t="s">
         <v>412</v>
       </c>
@@ -30916,7 +30920,7 @@
       </c>
       <c r="N657" s="36"/>
     </row>
-    <row r="658" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="658" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A658" s="138" t="s">
         <v>412</v>
       </c>
@@ -31046,7 +31050,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="661" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="661" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A661" s="138" t="s">
         <v>412</v>
       </c>
@@ -31088,7 +31092,7 @@
       </c>
       <c r="N661" s="36"/>
     </row>
-    <row r="662" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="662" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A662" s="138" t="s">
         <v>412</v>
       </c>
@@ -31130,7 +31134,7 @@
       </c>
       <c r="N662" s="36"/>
     </row>
-    <row r="663" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="663" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A663" s="138" t="s">
         <v>412</v>
       </c>
@@ -31172,7 +31176,7 @@
       </c>
       <c r="N663" s="36"/>
     </row>
-    <row r="664" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="664" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A664" s="138" t="s">
         <v>412</v>
       </c>
@@ -31214,7 +31218,7 @@
       </c>
       <c r="N664" s="36"/>
     </row>
-    <row r="665" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="665" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A665" s="138" t="s">
         <v>412</v>
       </c>
@@ -31256,7 +31260,7 @@
       </c>
       <c r="N665" s="36"/>
     </row>
-    <row r="666" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="666" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A666" s="138" t="s">
         <v>412</v>
       </c>
@@ -31342,7 +31346,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="668" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="668" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A668" s="138" t="s">
         <v>412</v>
       </c>
@@ -31384,7 +31388,7 @@
       </c>
       <c r="N668" s="36"/>
     </row>
-    <row r="669" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="669" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A669" s="138" t="s">
         <v>412</v>
       </c>
@@ -31426,7 +31430,7 @@
       </c>
       <c r="N669" s="36"/>
     </row>
-    <row r="670" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="670" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A670" s="138" t="s">
         <v>412</v>
       </c>
@@ -31468,7 +31472,7 @@
       </c>
       <c r="N670" s="36"/>
     </row>
-    <row r="671" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="671" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A671" s="138" t="s">
         <v>412</v>
       </c>
@@ -31510,7 +31514,7 @@
       </c>
       <c r="N671" s="36"/>
     </row>
-    <row r="672" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="672" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A672" s="138" t="s">
         <v>412</v>
       </c>
@@ -31552,7 +31556,7 @@
       </c>
       <c r="N672" s="36"/>
     </row>
-    <row r="673" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="673" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A673" s="138" t="s">
         <v>412</v>
       </c>
@@ -31638,7 +31642,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="675" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="675" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A675" s="138" t="s">
         <v>412</v>
       </c>
@@ -31680,7 +31684,7 @@
       </c>
       <c r="N675" s="36"/>
     </row>
-    <row r="676" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="676" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A676" s="138" t="s">
         <v>412</v>
       </c>
@@ -31722,7 +31726,7 @@
       </c>
       <c r="N676" s="36"/>
     </row>
-    <row r="677" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="677" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A677" s="138" t="s">
         <v>412</v>
       </c>
@@ -31764,7 +31768,7 @@
       </c>
       <c r="N677" s="36"/>
     </row>
-    <row r="678" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="678" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A678" s="138" t="s">
         <v>412</v>
       </c>
@@ -31806,7 +31810,7 @@
       </c>
       <c r="N678" s="36"/>
     </row>
-    <row r="679" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="679" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A679" s="138" t="s">
         <v>412</v>
       </c>
@@ -31848,7 +31852,7 @@
       </c>
       <c r="N679" s="36"/>
     </row>
-    <row r="680" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="680" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A680" s="138" t="s">
         <v>412</v>
       </c>
@@ -31890,7 +31894,7 @@
       </c>
       <c r="N680" s="36"/>
     </row>
-    <row r="681" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="681" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A681" s="138" t="s">
         <v>412</v>
       </c>
@@ -31934,7 +31938,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="682" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="682" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A682" s="138" t="s">
         <v>412</v>
       </c>
@@ -31978,7 +31982,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="683" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="683" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A683" s="138" t="s">
         <v>412</v>
       </c>
@@ -32022,7 +32026,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="684" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="684" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A684" s="138" t="s">
         <v>412</v>
       </c>
@@ -32064,7 +32068,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="685" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="685" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A685" s="138" t="s">
         <v>412</v>
       </c>
@@ -32108,7 +32112,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="686" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="686" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A686" s="138" t="s">
         <v>412</v>
       </c>
@@ -32152,7 +32156,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="687" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="687" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A687" s="138" t="s">
         <v>412</v>
       </c>
@@ -32196,7 +32200,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="688" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="688" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A688" s="138" t="s">
         <v>412</v>
       </c>
@@ -32238,7 +32242,7 @@
       </c>
       <c r="N688" s="36"/>
     </row>
-    <row r="689" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="689" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A689" s="138" t="s">
         <v>412</v>
       </c>
@@ -32280,7 +32284,7 @@
       </c>
       <c r="N689" s="36"/>
     </row>
-    <row r="690" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="690" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A690" s="138" t="s">
         <v>412</v>
       </c>
@@ -32322,7 +32326,7 @@
       </c>
       <c r="N690" s="67"/>
     </row>
-    <row r="691" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="691" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A691" s="138" t="s">
         <v>412</v>
       </c>
@@ -32364,7 +32368,7 @@
       </c>
       <c r="N691" s="36"/>
     </row>
-    <row r="692" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="692" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A692" s="138" t="s">
         <v>412</v>
       </c>
@@ -32406,7 +32410,7 @@
       </c>
       <c r="N692" s="36"/>
     </row>
-    <row r="693" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="693" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A693" s="138" t="s">
         <v>412</v>
       </c>
@@ -32448,7 +32452,7 @@
       </c>
       <c r="N693" s="36"/>
     </row>
-    <row r="694" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="694" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A694" s="138" t="s">
         <v>412</v>
       </c>
@@ -32490,7 +32494,7 @@
       </c>
       <c r="N694" s="36"/>
     </row>
-    <row r="695" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="695" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A695" s="138" t="s">
         <v>412</v>
       </c>
@@ -32532,7 +32536,7 @@
       </c>
       <c r="N695" s="36"/>
     </row>
-    <row r="696" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="696" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A696" s="138" t="s">
         <v>412</v>
       </c>
@@ -32574,7 +32578,7 @@
       </c>
       <c r="N696" s="36"/>
     </row>
-    <row r="697" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="697" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A697" s="138" t="s">
         <v>412</v>
       </c>
@@ -32616,7 +32620,7 @@
       </c>
       <c r="N697" s="36"/>
     </row>
-    <row r="698" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="698" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A698" s="138" t="s">
         <v>412</v>
       </c>
@@ -32658,7 +32662,7 @@
       </c>
       <c r="N698" s="36"/>
     </row>
-    <row r="699" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="699" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A699" s="138" t="s">
         <v>412</v>
       </c>
@@ -32700,7 +32704,7 @@
       </c>
       <c r="N699" s="36"/>
     </row>
-    <row r="700" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="700" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A700" s="138" t="s">
         <v>412</v>
       </c>
@@ -32742,7 +32746,7 @@
       </c>
       <c r="N700" s="36"/>
     </row>
-    <row r="701" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="701" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A701" s="138" t="s">
         <v>412</v>
       </c>
@@ -32784,7 +32788,7 @@
       </c>
       <c r="N701" s="36"/>
     </row>
-    <row r="702" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="702" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A702" s="138" t="s">
         <v>412</v>
       </c>
@@ -32826,7 +32830,7 @@
       </c>
       <c r="N702" s="36"/>
     </row>
-    <row r="703" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="703" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A703" s="138" t="s">
         <v>412</v>
       </c>
@@ -32868,7 +32872,7 @@
       </c>
       <c r="N703" s="36"/>
     </row>
-    <row r="704" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="704" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A704" s="138" t="s">
         <v>412</v>
       </c>
@@ -32910,7 +32914,7 @@
       </c>
       <c r="N704" s="36"/>
     </row>
-    <row r="705" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="705" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A705" s="138" t="s">
         <v>412</v>
       </c>
@@ -32952,7 +32956,7 @@
       </c>
       <c r="N705" s="36"/>
     </row>
-    <row r="706" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="706" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A706" s="138" t="s">
         <v>412</v>
       </c>
@@ -32994,7 +32998,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="707" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="707" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A707" s="138" t="s">
         <v>412</v>
       </c>
@@ -33036,7 +33040,7 @@
       </c>
       <c r="N707" s="36"/>
     </row>
-    <row r="708" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="708" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A708" s="138" t="s">
         <v>412</v>
       </c>
@@ -33078,7 +33082,7 @@
       </c>
       <c r="N708" s="36"/>
     </row>
-    <row r="709" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="709" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A709" s="138" t="s">
         <v>412</v>
       </c>
@@ -33120,7 +33124,7 @@
       </c>
       <c r="N709" s="36"/>
     </row>
-    <row r="710" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="710" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A710" s="138" t="s">
         <v>412</v>
       </c>
@@ -33162,7 +33166,7 @@
       </c>
       <c r="N710" s="36"/>
     </row>
-    <row r="711" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="711" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A711" s="138" t="s">
         <v>412</v>
       </c>
@@ -33204,7 +33208,7 @@
       </c>
       <c r="N711" s="36"/>
     </row>
-    <row r="712" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="712" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A712" s="138" t="s">
         <v>412</v>
       </c>
@@ -33334,7 +33338,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="715" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="715" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A715" s="138" t="s">
         <v>412</v>
       </c>
@@ -33378,7 +33382,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="716" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="716" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A716" s="138" t="s">
         <v>412</v>
       </c>
@@ -33420,7 +33424,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="717" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="717" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A717" s="138" t="s">
         <v>412</v>
       </c>
@@ -33464,7 +33468,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="718" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="718" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A718" s="138" t="s">
         <v>412</v>
       </c>
@@ -33552,7 +33556,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="720" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="720" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A720" s="138" t="s">
         <v>412</v>
       </c>
@@ -33684,7 +33688,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="723" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="723" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A723" s="138" t="s">
         <v>412</v>
       </c>
@@ -33726,7 +33730,7 @@
       </c>
       <c r="N723" s="36"/>
     </row>
-    <row r="724" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="724" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A724" s="138" t="s">
         <v>412</v>
       </c>
@@ -33768,7 +33772,7 @@
       </c>
       <c r="N724" s="36"/>
     </row>
-    <row r="725" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="725" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A725" s="138" t="s">
         <v>412</v>
       </c>
@@ -33810,7 +33814,7 @@
       </c>
       <c r="N725" s="36"/>
     </row>
-    <row r="726" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="726" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A726" s="138" t="s">
         <v>412</v>
       </c>
@@ -33852,7 +33856,7 @@
       </c>
       <c r="N726" s="36"/>
     </row>
-    <row r="727" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="727" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A727" s="138" t="s">
         <v>412</v>
       </c>
@@ -33894,7 +33898,7 @@
       </c>
       <c r="N727" s="36"/>
     </row>
-    <row r="728" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="728" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A728" s="138" t="s">
         <v>412</v>
       </c>
@@ -34024,7 +34028,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="731" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="731" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A731" s="138" t="s">
         <v>412</v>
       </c>
@@ -34066,7 +34070,7 @@
       </c>
       <c r="N731" s="36"/>
     </row>
-    <row r="732" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="732" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A732" s="138" t="s">
         <v>412</v>
       </c>
@@ -34108,7 +34112,7 @@
       </c>
       <c r="N732" s="36"/>
     </row>
-    <row r="733" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="733" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A733" s="138" t="s">
         <v>412</v>
       </c>
@@ -34150,7 +34154,7 @@
       </c>
       <c r="N733" s="36"/>
     </row>
-    <row r="734" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="734" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A734" s="138" t="s">
         <v>412</v>
       </c>
@@ -34192,7 +34196,7 @@
       </c>
       <c r="N734" s="36"/>
     </row>
-    <row r="735" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="735" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A735" s="138" t="s">
         <v>412</v>
       </c>
@@ -34234,7 +34238,7 @@
       </c>
       <c r="N735" s="36"/>
     </row>
-    <row r="736" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="736" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A736" s="138" t="s">
         <v>412</v>
       </c>
@@ -34320,7 +34324,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="738" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="738" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A738" s="138" t="s">
         <v>412</v>
       </c>
@@ -34362,7 +34366,7 @@
       </c>
       <c r="N738" s="36"/>
     </row>
-    <row r="739" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="739" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A739" s="138" t="s">
         <v>412</v>
       </c>
@@ -34404,7 +34408,7 @@
       </c>
       <c r="N739" s="36"/>
     </row>
-    <row r="740" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="740" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A740" s="138" t="s">
         <v>412</v>
       </c>
@@ -34446,7 +34450,7 @@
       </c>
       <c r="N740" s="36"/>
     </row>
-    <row r="741" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="741" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A741" s="138" t="s">
         <v>412</v>
       </c>
@@ -34488,7 +34492,7 @@
       </c>
       <c r="N741" s="36"/>
     </row>
-    <row r="742" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="742" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A742" s="138" t="s">
         <v>412</v>
       </c>
@@ -34530,7 +34534,7 @@
       </c>
       <c r="N742" s="36"/>
     </row>
-    <row r="743" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="743" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A743" s="138" t="s">
         <v>412</v>
       </c>
@@ -34616,7 +34620,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="745" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="745" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A745" s="138" t="s">
         <v>412</v>
       </c>
@@ -34658,7 +34662,7 @@
       </c>
       <c r="N745" s="36"/>
     </row>
-    <row r="746" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="746" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A746" s="138" t="s">
         <v>412</v>
       </c>
@@ -34700,7 +34704,7 @@
       </c>
       <c r="N746" s="36"/>
     </row>
-    <row r="747" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="747" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A747" s="138" t="s">
         <v>412</v>
       </c>
@@ -34742,7 +34746,7 @@
       </c>
       <c r="N747" s="67"/>
     </row>
-    <row r="748" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="748" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A748" s="138" t="s">
         <v>412</v>
       </c>
@@ -34784,7 +34788,7 @@
       </c>
       <c r="N748" s="36"/>
     </row>
-    <row r="749" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="749" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A749" s="138" t="s">
         <v>412</v>
       </c>
@@ -34826,7 +34830,7 @@
       </c>
       <c r="N749" s="36"/>
     </row>
-    <row r="750" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="750" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A750" s="138" t="s">
         <v>412</v>
       </c>
@@ -34868,7 +34872,7 @@
       </c>
       <c r="N750" s="36"/>
     </row>
-    <row r="751" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="751" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A751" s="138" t="s">
         <v>412</v>
       </c>
@@ -34912,7 +34916,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="752" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="752" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A752" s="138" t="s">
         <v>412</v>
       </c>
@@ -34956,7 +34960,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="753" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="753" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A753" s="138" t="s">
         <v>412</v>
       </c>
@@ -35000,7 +35004,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="754" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="754" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A754" s="138" t="s">
         <v>412</v>
       </c>
@@ -35042,7 +35046,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="755" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="755" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A755" s="138" t="s">
         <v>412</v>
       </c>
@@ -35086,7 +35090,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="756" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="756" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A756" s="138" t="s">
         <v>412</v>
       </c>
@@ -35130,7 +35134,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="757" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="757" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A757" s="138" t="s">
         <v>412</v>
       </c>
@@ -35174,7 +35178,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="758" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="758" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A758" s="138" t="s">
         <v>412</v>
       </c>
@@ -35218,7 +35222,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="759" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="759" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A759" s="138" t="s">
         <v>412</v>
       </c>
@@ -35262,7 +35266,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="760" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="760" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A760" s="138" t="s">
         <v>412</v>
       </c>
@@ -35306,7 +35310,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="761" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="761" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A761" s="138" t="s">
         <v>412</v>
       </c>
@@ -35350,7 +35354,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="762" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="762" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A762" s="138" t="s">
         <v>412</v>
       </c>
@@ -35394,7 +35398,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="763" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="763" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A763" s="138" t="s">
         <v>412</v>
       </c>
@@ -35438,7 +35442,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="764" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="764" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A764" s="138" t="s">
         <v>412</v>
       </c>
@@ -35482,7 +35486,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="765" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="765" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A765" s="138" t="s">
         <v>412</v>
       </c>
@@ -35526,7 +35530,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="766" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="766" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A766" s="138" t="s">
         <v>412</v>
       </c>
@@ -35570,7 +35574,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="767" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="767" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A767" s="138" t="s">
         <v>412</v>
       </c>
@@ -35614,7 +35618,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="768" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="768" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A768" s="138" t="s">
         <v>412</v>
       </c>
@@ -35656,7 +35660,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="769" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="769" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A769" s="138" t="s">
         <v>412</v>
       </c>
@@ -35700,7 +35704,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="770" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="770" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A770" s="138" t="s">
         <v>412</v>
       </c>
@@ -35744,7 +35748,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="771" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="771" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A771" s="138" t="s">
         <v>412</v>
       </c>
@@ -35788,7 +35792,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="772" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="772" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A772" s="138" t="s">
         <v>412</v>
       </c>
@@ -35918,7 +35922,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="775" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="775" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A775" s="138" t="s">
         <v>412</v>
       </c>
@@ -35960,7 +35964,7 @@
       </c>
       <c r="N775" s="36"/>
     </row>
-    <row r="776" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="776" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A776" s="138" t="s">
         <v>412</v>
       </c>
@@ -36002,7 +36006,7 @@
       </c>
       <c r="N776" s="36"/>
     </row>
-    <row r="777" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="777" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A777" s="138" t="s">
         <v>412</v>
       </c>
@@ -36044,7 +36048,7 @@
       </c>
       <c r="N777" s="67"/>
     </row>
-    <row r="778" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="778" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A778" s="138" t="s">
         <v>412</v>
       </c>
@@ -36086,7 +36090,7 @@
       </c>
       <c r="N778" s="36"/>
     </row>
-    <row r="779" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="779" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A779" s="138" t="s">
         <v>412</v>
       </c>
@@ -36128,7 +36132,7 @@
       </c>
       <c r="N779" s="36"/>
     </row>
-    <row r="780" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="780" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A780" s="138" t="s">
         <v>412</v>
       </c>
@@ -36258,7 +36262,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="783" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="783" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A783" s="138" t="s">
         <v>412</v>
       </c>
@@ -36300,7 +36304,7 @@
       </c>
       <c r="N783" s="36"/>
     </row>
-    <row r="784" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="784" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A784" s="138" t="s">
         <v>412</v>
       </c>
@@ -36342,7 +36346,7 @@
       </c>
       <c r="N784" s="36"/>
     </row>
-    <row r="785" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="785" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A785" s="138" t="s">
         <v>412</v>
       </c>
@@ -36384,7 +36388,7 @@
       </c>
       <c r="N785" s="36"/>
     </row>
-    <row r="786" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="786" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A786" s="138" t="s">
         <v>412</v>
       </c>
@@ -36426,7 +36430,7 @@
       </c>
       <c r="N786" s="36"/>
     </row>
-    <row r="787" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="787" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A787" s="138" t="s">
         <v>412</v>
       </c>
@@ -36468,7 +36472,7 @@
       </c>
       <c r="N787" s="36"/>
     </row>
-    <row r="788" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="788" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A788" s="138" t="s">
         <v>412</v>
       </c>
@@ -36554,7 +36558,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="790" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="790" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A790" s="138" t="s">
         <v>412</v>
       </c>
@@ -36596,7 +36600,7 @@
       </c>
       <c r="N790" s="36"/>
     </row>
-    <row r="791" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="791" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A791" s="138" t="s">
         <v>412</v>
       </c>
@@ -36638,7 +36642,7 @@
       </c>
       <c r="N791" s="36"/>
     </row>
-    <row r="792" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="792" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A792" s="138" t="s">
         <v>412</v>
       </c>
@@ -36680,7 +36684,7 @@
       </c>
       <c r="N792" s="36"/>
     </row>
-    <row r="793" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="793" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A793" s="138" t="s">
         <v>412</v>
       </c>
@@ -36722,7 +36726,7 @@
       </c>
       <c r="N793" s="36"/>
     </row>
-    <row r="794" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="794" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A794" s="138" t="s">
         <v>412</v>
       </c>
@@ -36764,7 +36768,7 @@
       </c>
       <c r="N794" s="36"/>
     </row>
-    <row r="795" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="795" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A795" s="138" t="s">
         <v>412</v>
       </c>
@@ -36806,7 +36810,7 @@
       </c>
       <c r="N795" s="36"/>
     </row>
-    <row r="796" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="796" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A796" s="138" t="s">
         <v>412</v>
       </c>
@@ -36850,7 +36854,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="797" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="797" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A797" s="138" t="s">
         <v>412</v>
       </c>
@@ -36892,7 +36896,7 @@
       </c>
       <c r="N797" s="36"/>
     </row>
-    <row r="798" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="798" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A798" s="138" t="s">
         <v>412</v>
       </c>
@@ -36934,7 +36938,7 @@
       </c>
       <c r="N798" s="36"/>
     </row>
-    <row r="799" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="799" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A799" s="138" t="s">
         <v>412</v>
       </c>
@@ -36976,7 +36980,7 @@
       </c>
       <c r="N799" s="36"/>
     </row>
-    <row r="800" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="800" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A800" s="138" t="s">
         <v>412</v>
       </c>
@@ -37018,7 +37022,7 @@
       </c>
       <c r="N800" s="36"/>
     </row>
-    <row r="801" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="801" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A801" s="138" t="s">
         <v>412</v>
       </c>
@@ -37060,7 +37064,7 @@
       </c>
       <c r="N801" s="36"/>
     </row>
-    <row r="802" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="802" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A802" s="138" t="s">
         <v>412</v>
       </c>
@@ -37074,7 +37078,7 @@
         <v>127</v>
       </c>
       <c r="E802" s="15">
-        <v>45411</v>
+        <v>45413</v>
       </c>
       <c r="F802" s="16">
         <v>0.625</v>
@@ -37141,6 +37145,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="d111bada-3e6f-4186-af72-321f17a92816">
+      <UserInfo>
+        <DisplayName>Tony Furnell</DisplayName>
+        <AccountId>21</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010047D52C2EB712F341B0DF2D9ED5D9506A" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f60e02c0650e9ea2000e83e55453fc7f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1f086a82-432d-45e9-9ca6-8ca760156e0b" xmlns:ns3="d111bada-3e6f-4186-af72-321f17a92816" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="897166873492abbc78f80725dcffa27c" ns2:_="" ns3:_="">
     <xsd:import namespace="1f086a82-432d-45e9-9ca6-8ca760156e0b"/>
@@ -37319,20 +37337,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="d111bada-3e6f-4186-af72-321f17a92816">
-      <UserInfo>
-        <DisplayName>Tony Furnell</DisplayName>
-        <AccountId>21</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFC73EDA-6B2F-4B5B-858E-6AD4B6E182A8}">
   <ds:schemaRefs>
@@ -37342,6 +37346,16 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{836137F5-2A5A-4F0D-935E-C8DB69844C45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d111bada-3e6f-4186-af72-321f17a92816"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D336B7E-CD9A-40DA-B016-D0811386B08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -37358,14 +37372,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{836137F5-2A5A-4F0D-935E-C8DB69844C45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d111bada-3e6f-4186-af72-321f17a92816"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>